<commit_message>
Retirement Account Types. Fixes for "How Much You Need" and "How Long Does It Take".
</commit_message>
<xml_diff>
--- a/content/finance/2021/2021-06-03-how-long-does-it-take/files/time-to-retirement.xlsx
+++ b/content/finance/2021/2021-06-03-how-long-does-it-take/files/time-to-retirement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\blog\content\finance\2021\2021-06-03-how-long-does-it-take\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0291DB-8342-459D-B186-BA1DC41E765D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7FEA44-BB77-4ED0-9312-0117A07C0110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7635" yWindow="1290" windowWidth="28800" windowHeight="18960" firstSheet="1" activeTab="2" xr2:uid="{08A55DC8-DC65-4D69-9AFB-D59CCB65EDF1}"/>
+    <workbookView xWindow="7665" yWindow="0" windowWidth="16770" windowHeight="15600" firstSheet="1" activeTab="3" xr2:uid="{08A55DC8-DC65-4D69-9AFB-D59CCB65EDF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId1"/>
@@ -93,9 +93,9 @@
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -139,15 +139,15 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1258,7 +1258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D469C10-986A-4BFE-8ABF-32EAB627C638}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <f>B2*Rate</f>
+        <f t="shared" ref="C2:C37" si="0">B2*Rate</f>
         <v>0</v>
       </c>
       <c r="D2" s="2">
@@ -1316,14 +1316,14 @@
         <v>10000</v>
       </c>
       <c r="C3" s="2">
-        <f>B3*Rate</f>
+        <f t="shared" si="0"/>
         <v>704</v>
       </c>
       <c r="D3" s="2">
         <v>10000</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E29" si="0">B3+C3+D3</f>
+        <f t="shared" ref="E3:E29" si="1">B3+C3+D3</f>
         <v>20704</v>
       </c>
     </row>
@@ -1332,18 +1332,18 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <f t="shared" ref="B4:B29" si="1">E3</f>
+        <f t="shared" ref="B4:B29" si="2">E3</f>
         <v>20704</v>
       </c>
       <c r="C4" s="2">
-        <f>B4*Rate</f>
+        <f t="shared" si="0"/>
         <v>1457.5616</v>
       </c>
       <c r="D4" s="2">
         <v>10000</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32161.561600000001</v>
       </c>
     </row>
@@ -1352,18 +1352,18 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32161.561600000001</v>
       </c>
       <c r="C5" s="2">
-        <f>B5*Rate</f>
+        <f t="shared" si="0"/>
         <v>2264.1739366400002</v>
       </c>
       <c r="D5" s="2">
         <v>10000</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44425.735536640001</v>
       </c>
     </row>
@@ -1372,18 +1372,18 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44425.735536640001</v>
       </c>
       <c r="C6" s="2">
-        <f>B6*Rate</f>
+        <f t="shared" si="0"/>
         <v>3127.5717817794562</v>
       </c>
       <c r="D6" s="2">
         <v>10000</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57553.307318419458</v>
       </c>
     </row>
@@ -1392,18 +1392,18 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>57553.307318419458</v>
       </c>
       <c r="C7" s="2">
-        <f>B7*Rate</f>
+        <f t="shared" si="0"/>
         <v>4051.7528352167301</v>
       </c>
       <c r="D7" s="2">
         <v>10000</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71605.060153636179</v>
       </c>
     </row>
@@ -1412,18 +1412,18 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71605.060153636179</v>
       </c>
       <c r="C8" s="2">
-        <f>B8*Rate</f>
+        <f t="shared" si="0"/>
         <v>5040.996234815987</v>
       </c>
       <c r="D8" s="2">
         <v>10000</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86646.056388452169</v>
       </c>
     </row>
@@ -1432,18 +1432,18 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>86646.056388452169</v>
       </c>
       <c r="C9" s="2">
-        <f>B9*Rate</f>
+        <f t="shared" si="0"/>
         <v>6099.8823697470334</v>
       </c>
       <c r="D9" s="2">
         <v>10000</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>102745.93875819921</v>
       </c>
     </row>
@@ -1452,18 +1452,18 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102745.93875819921</v>
       </c>
       <c r="C10" s="2">
-        <f>B10*Rate</f>
+        <f t="shared" si="0"/>
         <v>7233.3140885772245</v>
       </c>
       <c r="D10" s="2">
         <v>10000</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>119979.25284677644</v>
       </c>
     </row>
@@ -1472,18 +1472,18 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119979.25284677644</v>
       </c>
       <c r="C11" s="2">
-        <f>B11*Rate</f>
+        <f t="shared" si="0"/>
         <v>8446.5394004130612</v>
       </c>
       <c r="D11" s="2">
         <v>10000</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>138425.7922471895</v>
       </c>
     </row>
@@ -1492,18 +1492,18 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>138425.7922471895</v>
       </c>
       <c r="C12" s="2">
-        <f>B12*Rate</f>
+        <f t="shared" si="0"/>
         <v>9745.1757742021418</v>
       </c>
       <c r="D12" s="2">
         <v>10000</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>158170.96802139163</v>
       </c>
     </row>
@@ -1512,18 +1512,18 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>158170.96802139163</v>
       </c>
       <c r="C13" s="2">
-        <f>B13*Rate</f>
+        <f t="shared" si="0"/>
         <v>11135.236148705972</v>
       </c>
       <c r="D13" s="2">
         <v>10000</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>179306.2041700976</v>
       </c>
     </row>
@@ -1532,18 +1532,18 @@
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>179306.2041700976</v>
       </c>
       <c r="C14" s="2">
-        <f>B14*Rate</f>
+        <f t="shared" si="0"/>
         <v>12623.156773574872</v>
       </c>
       <c r="D14" s="2">
         <v>10000</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>201929.36094367248</v>
       </c>
     </row>
@@ -1552,18 +1552,18 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>201929.36094367248</v>
       </c>
       <c r="C15" s="2">
-        <f>B15*Rate</f>
+        <f t="shared" si="0"/>
         <v>14215.827010434543</v>
       </c>
       <c r="D15" s="2">
         <v>10000</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>226145.18795410701</v>
       </c>
     </row>
@@ -1572,18 +1572,18 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>226145.18795410701</v>
       </c>
       <c r="C16" s="2">
-        <f>B16*Rate</f>
+        <f t="shared" si="0"/>
         <v>15920.621231969135</v>
       </c>
       <c r="D16" s="2">
         <v>10000</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252065.80918607613</v>
       </c>
     </row>
@@ -1592,18 +1592,18 @@
         <v>16</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>252065.80918607613</v>
       </c>
       <c r="C17" s="2">
-        <f>B17*Rate</f>
+        <f t="shared" si="0"/>
         <v>17745.432966699762</v>
       </c>
       <c r="D17" s="2">
         <v>10000</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>279811.24215277587</v>
       </c>
     </row>
@@ -1612,18 +1612,18 @@
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>279811.24215277587</v>
       </c>
       <c r="C18" s="2">
-        <f>B18*Rate</f>
+        <f t="shared" si="0"/>
         <v>19698.711447555423</v>
       </c>
       <c r="D18" s="2">
         <v>10000</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>309509.95360033127</v>
       </c>
     </row>
@@ -1632,18 +1632,18 @@
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>309509.95360033127</v>
       </c>
       <c r="C19" s="2">
-        <f>B19*Rate</f>
+        <f t="shared" si="0"/>
         <v>21789.500733463323</v>
       </c>
       <c r="D19" s="2">
         <v>10000</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>341299.45433379459</v>
       </c>
     </row>
@@ -1652,18 +1652,18 @@
         <v>19</v>
       </c>
       <c r="B20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>341299.45433379459</v>
       </c>
       <c r="C20" s="2">
-        <f>B20*Rate</f>
+        <f t="shared" si="0"/>
         <v>24027.48158509914</v>
       </c>
       <c r="D20" s="2">
         <v>10000</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>375326.93591889372</v>
       </c>
     </row>
@@ -1672,18 +1672,18 @@
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>375326.93591889372</v>
       </c>
       <c r="C21" s="2">
-        <f>B21*Rate</f>
+        <f t="shared" si="0"/>
         <v>26423.01628869012</v>
       </c>
       <c r="D21" s="2">
         <v>10000</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>411749.95220758382</v>
       </c>
     </row>
@@ -1692,18 +1692,18 @@
         <v>21</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>411749.95220758382</v>
       </c>
       <c r="C22" s="2">
-        <f>B22*Rate</f>
+        <f t="shared" si="0"/>
         <v>28987.196635413904</v>
       </c>
       <c r="D22" s="2">
         <v>10000</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>450737.14884299773</v>
       </c>
     </row>
@@ -1712,18 +1712,18 @@
         <v>22</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>450737.14884299773</v>
       </c>
       <c r="C23" s="2">
-        <f>B23*Rate</f>
+        <f t="shared" si="0"/>
         <v>31731.895278547043</v>
       </c>
       <c r="D23" s="2">
         <v>10000</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>492469.04412154475</v>
       </c>
     </row>
@@ -1732,18 +1732,18 @@
         <v>23</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>492469.04412154475</v>
       </c>
       <c r="C24" s="2">
-        <f>B24*Rate</f>
+        <f t="shared" si="0"/>
         <v>34669.820706156752</v>
       </c>
       <c r="D24" s="2">
         <v>10000</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>537138.86482770147</v>
       </c>
     </row>
@@ -1752,18 +1752,18 @@
         <v>24</v>
       </c>
       <c r="B25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>537138.86482770147</v>
       </c>
       <c r="C25" s="2">
-        <f>B25*Rate</f>
+        <f t="shared" si="0"/>
         <v>37814.576083870183</v>
       </c>
       <c r="D25" s="2">
         <v>10000</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>584953.44091157161</v>
       </c>
     </row>
@@ -1772,18 +1772,18 @@
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>584953.44091157161</v>
       </c>
       <c r="C26" s="2">
-        <f>B26*Rate</f>
+        <f t="shared" si="0"/>
         <v>41180.72224017464</v>
       </c>
       <c r="D26" s="2">
         <v>10000</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>636134.16315174627</v>
       </c>
     </row>
@@ -1792,18 +1792,18 @@
         <v>26</v>
       </c>
       <c r="B27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>636134.16315174627</v>
       </c>
       <c r="C27" s="2">
-        <f>B27*Rate</f>
+        <f t="shared" si="0"/>
         <v>44783.845085882938</v>
       </c>
       <c r="D27" s="2">
         <v>10000</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>690918.0082376292</v>
       </c>
     </row>
@@ -1812,18 +1812,18 @@
         <v>27</v>
       </c>
       <c r="B28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>690918.0082376292</v>
       </c>
       <c r="C28" s="2">
-        <f>B28*Rate</f>
+        <f t="shared" si="0"/>
         <v>48640.627779929098</v>
       </c>
       <c r="D28" s="2">
         <v>10000</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>749558.63601755828</v>
       </c>
     </row>
@@ -1832,18 +1832,18 @@
         <v>28</v>
       </c>
       <c r="B29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>749558.63601755828</v>
       </c>
       <c r="C29" s="2">
-        <f>B29*Rate</f>
+        <f t="shared" si="0"/>
         <v>52768.927975636107</v>
       </c>
       <c r="D29" s="2">
         <v>10000</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>812327.56399319437</v>
       </c>
     </row>
@@ -1852,18 +1852,18 @@
         <v>29</v>
       </c>
       <c r="B30" s="3">
-        <f t="shared" ref="B30:B37" si="2">E29</f>
+        <f t="shared" ref="B30:B37" si="3">E29</f>
         <v>812327.56399319437</v>
       </c>
       <c r="C30" s="2">
-        <f>B30*Rate</f>
+        <f t="shared" si="0"/>
         <v>57187.860505120887</v>
       </c>
       <c r="D30" s="2">
         <v>10000</v>
       </c>
       <c r="E30" s="3">
-        <f t="shared" ref="E30:E37" si="3">B30+C30+D30</f>
+        <f t="shared" ref="E30:E37" si="4">B30+C30+D30</f>
         <v>879515.4244983152</v>
       </c>
     </row>
@@ -1872,18 +1872,18 @@
         <v>30</v>
       </c>
       <c r="B31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>879515.4244983152</v>
       </c>
       <c r="C31" s="2">
-        <f>B31*Rate</f>
+        <f t="shared" si="0"/>
         <v>61917.885884681396</v>
       </c>
       <c r="D31" s="2">
         <v>10000</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>951433.31038299657</v>
       </c>
     </row>
@@ -1892,18 +1892,18 @@
         <v>31</v>
       </c>
       <c r="B32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>951433.31038299657</v>
       </c>
       <c r="C32" s="2">
-        <f>B32*Rate</f>
+        <f t="shared" si="0"/>
         <v>66980.90505096296</v>
       </c>
       <c r="D32" s="2">
         <v>10000</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1028414.2154339595</v>
       </c>
     </row>
@@ -1912,18 +1912,18 @@
         <v>32</v>
       </c>
       <c r="B33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1028414.2154339595</v>
       </c>
       <c r="C33" s="2">
-        <f>B33*Rate</f>
+        <f t="shared" si="0"/>
         <v>72400.360766550759</v>
       </c>
       <c r="D33" s="2">
         <v>10000</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1110814.5762005104</v>
       </c>
     </row>
@@ -1932,18 +1932,18 @@
         <v>33</v>
       </c>
       <c r="B34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1110814.5762005104</v>
       </c>
       <c r="C34" s="2">
-        <f>B34*Rate</f>
+        <f t="shared" si="0"/>
         <v>78201.34616451594</v>
       </c>
       <c r="D34" s="2">
         <v>10000</v>
       </c>
       <c r="E34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1199015.9223650263</v>
       </c>
     </row>
@@ -1952,18 +1952,18 @@
         <v>34</v>
       </c>
       <c r="B35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1199015.9223650263</v>
       </c>
       <c r="C35" s="2">
-        <f>B35*Rate</f>
+        <f t="shared" si="0"/>
         <v>84410.720934497862</v>
       </c>
       <c r="D35" s="2">
         <v>10000</v>
       </c>
       <c r="E35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1293426.6432995242</v>
       </c>
     </row>
@@ -1972,18 +1972,18 @@
         <v>35</v>
       </c>
       <c r="B36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1293426.6432995242</v>
       </c>
       <c r="C36" s="2">
-        <f>B36*Rate</f>
+        <f t="shared" si="0"/>
         <v>91057.235688286513</v>
       </c>
       <c r="D36" s="2">
         <v>10000</v>
       </c>
       <c r="E36" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1394483.8789878108</v>
       </c>
     </row>
@@ -1992,18 +1992,18 @@
         <v>36</v>
       </c>
       <c r="B37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1394483.8789878108</v>
       </c>
       <c r="C37" s="2">
-        <f>B37*Rate</f>
+        <f t="shared" si="0"/>
         <v>98171.665080741892</v>
       </c>
       <c r="D37" s="2">
         <v>10000</v>
       </c>
       <c r="E37" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1502655.5440685528</v>
       </c>
     </row>
@@ -2028,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609D0DC3-408F-4825-818E-ABABDDF14802}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2073,7 +2073,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <f>B2*Rate</f>
+        <f t="shared" ref="C2:C29" si="0">B2*Rate</f>
         <v>0</v>
       </c>
       <c r="D2" s="2">
@@ -2084,11 +2084,11 @@
         <v>10000</v>
       </c>
       <c r="F2" s="2">
-        <v>60000</v>
+        <v>59000</v>
       </c>
       <c r="G2" s="3">
-        <f>F2*YearsOfSpending</f>
-        <v>1500000</v>
+        <f t="shared" ref="G2:G29" si="1">F2*YearsOfSpending</f>
+        <v>1475000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2100,22 +2100,22 @@
         <v>10000</v>
       </c>
       <c r="C3" s="2">
-        <f>B3*Rate</f>
+        <f t="shared" si="0"/>
         <v>704</v>
       </c>
       <c r="D3" s="2">
         <v>10500</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E51" si="0">B3+C3+D3</f>
+        <f t="shared" ref="E3:E29" si="2">B3+C3+D3</f>
         <v>21204</v>
       </c>
       <c r="F3" s="2">
-        <v>59500</v>
+        <v>58500</v>
       </c>
       <c r="G3" s="3">
-        <f>F3*YearsOfSpending</f>
-        <v>1487500</v>
+        <f t="shared" si="1"/>
+        <v>1462500</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2123,26 +2123,26 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <f t="shared" ref="B4:B51" si="1">E3</f>
+        <f t="shared" ref="B4:B29" si="3">E3</f>
         <v>21204</v>
       </c>
       <c r="C4" s="2">
-        <f>B4*Rate</f>
+        <f t="shared" si="0"/>
         <v>1492.7616</v>
       </c>
       <c r="D4" s="2">
         <v>11000</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>33696.761599999998</v>
       </c>
       <c r="F4" s="2">
-        <v>59000</v>
+        <v>58000</v>
       </c>
       <c r="G4" s="3">
-        <f>F4*YearsOfSpending</f>
-        <v>1475000</v>
+        <f t="shared" si="1"/>
+        <v>1450000</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2150,26 +2150,26 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>33696.761599999998</v>
       </c>
       <c r="C5" s="2">
-        <f>B5*Rate</f>
+        <f t="shared" si="0"/>
         <v>2372.25201664</v>
       </c>
       <c r="D5" s="2">
         <v>11500</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>47569.013616639997</v>
       </c>
       <c r="F5" s="2">
-        <v>58500</v>
+        <v>57500</v>
       </c>
       <c r="G5" s="3">
-        <f>F5*YearsOfSpending</f>
-        <v>1462500</v>
+        <f t="shared" si="1"/>
+        <v>1437500</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2177,26 +2177,26 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>47569.013616639997</v>
       </c>
       <c r="C6" s="2">
-        <f>B6*Rate</f>
+        <f t="shared" si="0"/>
         <v>3348.8585586114559</v>
       </c>
       <c r="D6" s="2">
         <v>12000</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>62917.872175251454</v>
       </c>
       <c r="F6" s="2">
-        <v>58000</v>
+        <v>57000</v>
       </c>
       <c r="G6" s="3">
-        <f>F6*YearsOfSpending</f>
-        <v>1450000</v>
+        <f t="shared" si="1"/>
+        <v>1425000</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2204,26 +2204,26 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>62917.872175251454</v>
       </c>
       <c r="C7" s="2">
-        <f>B7*Rate</f>
+        <f t="shared" si="0"/>
         <v>4429.4182011377025</v>
       </c>
       <c r="D7" s="2">
         <v>12500</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>79847.290376389152</v>
       </c>
       <c r="F7" s="2">
-        <v>57500</v>
+        <v>56500</v>
       </c>
       <c r="G7" s="3">
-        <f>F7*YearsOfSpending</f>
-        <v>1437500</v>
+        <f t="shared" si="1"/>
+        <v>1412500</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2231,26 +2231,26 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>79847.290376389152</v>
       </c>
       <c r="C8" s="2">
-        <f>B8*Rate</f>
+        <f t="shared" si="0"/>
         <v>5621.2492424977963</v>
       </c>
       <c r="D8" s="2">
         <v>13000</v>
       </c>
       <c r="E8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>98468.539618886949</v>
       </c>
       <c r="F8" s="2">
-        <v>57000</v>
+        <v>56000</v>
       </c>
       <c r="G8" s="3">
-        <f>F8*YearsOfSpending</f>
-        <v>1425000</v>
+        <f t="shared" si="1"/>
+        <v>1400000</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2258,26 +2258,26 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>98468.539618886949</v>
       </c>
       <c r="C9" s="2">
-        <f>B9*Rate</f>
+        <f t="shared" si="0"/>
         <v>6932.1851891696415</v>
       </c>
       <c r="D9" s="2">
         <v>13500</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>118900.72480805659</v>
       </c>
       <c r="F9" s="2">
-        <v>56500</v>
+        <v>55500</v>
       </c>
       <c r="G9" s="3">
-        <f>F9*YearsOfSpending</f>
-        <v>1412500</v>
+        <f t="shared" si="1"/>
+        <v>1387500</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2285,26 +2285,26 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>118900.72480805659</v>
       </c>
       <c r="C10" s="2">
-        <f>B10*Rate</f>
+        <f t="shared" si="0"/>
         <v>8370.6110264871841</v>
       </c>
       <c r="D10" s="2">
         <v>14000</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>141271.33583454377</v>
       </c>
       <c r="F10" s="2">
-        <v>56000</v>
+        <v>55000</v>
       </c>
       <c r="G10" s="3">
-        <f>F10*YearsOfSpending</f>
-        <v>1400000</v>
+        <f t="shared" si="1"/>
+        <v>1375000</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2312,26 +2312,26 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>141271.33583454377</v>
       </c>
       <c r="C11" s="2">
-        <f>B11*Rate</f>
+        <f t="shared" si="0"/>
         <v>9945.502042751883</v>
       </c>
       <c r="D11" s="2">
         <v>14500</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>165716.83787729565</v>
       </c>
       <c r="F11" s="2">
-        <v>55500</v>
+        <v>54500</v>
       </c>
       <c r="G11" s="3">
-        <f>F11*YearsOfSpending</f>
-        <v>1387500</v>
+        <f t="shared" si="1"/>
+        <v>1362500</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2339,26 +2339,26 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>165716.83787729565</v>
       </c>
       <c r="C12" s="2">
-        <f>B12*Rate</f>
+        <f t="shared" si="0"/>
         <v>11666.465386561615</v>
       </c>
       <c r="D12" s="2">
         <v>15000</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>192383.30326385726</v>
       </c>
       <c r="F12" s="2">
-        <v>55000</v>
+        <v>54000</v>
       </c>
       <c r="G12" s="3">
-        <f>F12*YearsOfSpending</f>
-        <v>1375000</v>
+        <f t="shared" si="1"/>
+        <v>1350000</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2366,26 +2366,26 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>192383.30326385726</v>
       </c>
       <c r="C13" s="2">
-        <f>B13*Rate</f>
+        <f t="shared" si="0"/>
         <v>13543.784549775552</v>
       </c>
       <c r="D13" s="2">
         <v>15500</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>221427.08781363282</v>
       </c>
       <c r="F13" s="2">
-        <v>54500</v>
+        <v>53500</v>
       </c>
       <c r="G13" s="3">
-        <f>F13*YearsOfSpending</f>
-        <v>1362500</v>
+        <f t="shared" si="1"/>
+        <v>1337500</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2393,26 +2393,26 @@
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>221427.08781363282</v>
       </c>
       <c r="C14" s="2">
-        <f>B14*Rate</f>
+        <f t="shared" si="0"/>
         <v>15588.466982079752</v>
       </c>
       <c r="D14" s="2">
         <v>16000</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>253015.55479571258</v>
       </c>
       <c r="F14" s="2">
-        <v>54000</v>
+        <v>53000</v>
       </c>
       <c r="G14" s="3">
-        <f>F14*YearsOfSpending</f>
-        <v>1350000</v>
+        <f t="shared" si="1"/>
+        <v>1325000</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2420,26 +2420,26 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>253015.55479571258</v>
       </c>
       <c r="C15" s="2">
-        <f>B15*Rate</f>
+        <f t="shared" si="0"/>
         <v>17812.295057618168</v>
       </c>
       <c r="D15" s="2">
         <v>16500</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>287327.84985333076</v>
       </c>
       <c r="F15" s="2">
-        <v>53500</v>
+        <v>52500</v>
       </c>
       <c r="G15" s="3">
-        <f>F15*YearsOfSpending</f>
-        <v>1337500</v>
+        <f t="shared" si="1"/>
+        <v>1312500</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2447,26 +2447,26 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>287327.84985333076</v>
       </c>
       <c r="C16" s="2">
-        <f>B16*Rate</f>
+        <f t="shared" si="0"/>
         <v>20227.880629674488</v>
       </c>
       <c r="D16" s="2">
         <v>17000</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>324555.73048300523</v>
       </c>
       <c r="F16" s="2">
-        <v>53000</v>
+        <v>52000</v>
       </c>
       <c r="G16" s="3">
-        <f>F16*YearsOfSpending</f>
-        <v>1325000</v>
+        <f t="shared" si="1"/>
+        <v>1300000</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2474,26 +2474,26 @@
         <v>16</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>324555.73048300523</v>
       </c>
       <c r="C17" s="2">
-        <f>B17*Rate</f>
+        <f t="shared" si="0"/>
         <v>22848.723426003569</v>
       </c>
       <c r="D17" s="2">
         <v>17500</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>364904.45390900882</v>
       </c>
       <c r="F17" s="2">
-        <v>52500</v>
+        <v>51500</v>
       </c>
       <c r="G17" s="3">
-        <f>F17*YearsOfSpending</f>
-        <v>1312500</v>
+        <f t="shared" si="1"/>
+        <v>1287500</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2501,26 +2501,26 @@
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>364904.45390900882</v>
       </c>
       <c r="C18" s="2">
-        <f>B18*Rate</f>
+        <f t="shared" si="0"/>
         <v>25689.273555194224</v>
       </c>
       <c r="D18" s="2">
         <v>18000</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>408593.72746420302</v>
       </c>
       <c r="F18" s="2">
-        <v>52000</v>
+        <v>51000</v>
       </c>
       <c r="G18" s="3">
-        <f>F18*YearsOfSpending</f>
-        <v>1300000</v>
+        <f t="shared" si="1"/>
+        <v>1275000</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2528,26 +2528,26 @@
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>408593.72746420302</v>
       </c>
       <c r="C19" s="2">
-        <f>B19*Rate</f>
+        <f t="shared" si="0"/>
         <v>28764.998413479894</v>
       </c>
       <c r="D19" s="2">
         <v>18500</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>455858.72587768291</v>
       </c>
       <c r="F19" s="2">
-        <v>51500</v>
+        <v>50500</v>
       </c>
       <c r="G19" s="3">
-        <f>F19*YearsOfSpending</f>
-        <v>1287500</v>
+        <f t="shared" si="1"/>
+        <v>1262500</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2555,26 +2555,26 @@
         <v>19</v>
       </c>
       <c r="B20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>455858.72587768291</v>
       </c>
       <c r="C20" s="2">
-        <f>B20*Rate</f>
+        <f t="shared" si="0"/>
         <v>32092.454301788879</v>
       </c>
       <c r="D20" s="2">
         <v>19000</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>506951.18017947179</v>
       </c>
       <c r="F20" s="2">
-        <v>51000</v>
+        <v>50000</v>
       </c>
       <c r="G20" s="3">
-        <f>F20*YearsOfSpending</f>
-        <v>1275000</v>
+        <f t="shared" si="1"/>
+        <v>1250000</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2582,26 +2582,26 @@
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>506951.18017947179</v>
       </c>
       <c r="C21" s="2">
-        <f>B21*Rate</f>
+        <f t="shared" si="0"/>
         <v>35689.363084634817</v>
       </c>
       <c r="D21" s="2">
         <v>19500</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>562140.54326410661</v>
       </c>
       <c r="F21" s="2">
-        <v>50500</v>
+        <v>49500</v>
       </c>
       <c r="G21" s="3">
-        <f>F21*YearsOfSpending</f>
-        <v>1262500</v>
+        <f t="shared" si="1"/>
+        <v>1237500</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2609,26 +2609,26 @@
         <v>21</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>562140.54326410661</v>
       </c>
       <c r="C22" s="2">
-        <f>B22*Rate</f>
+        <f t="shared" si="0"/>
         <v>39574.694245793107</v>
       </c>
       <c r="D22" s="2">
         <v>20000</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>621715.23750989977</v>
       </c>
       <c r="F22" s="2">
-        <v>50000</v>
+        <v>49000</v>
       </c>
       <c r="G22" s="3">
-        <f>F22*YearsOfSpending</f>
-        <v>1250000</v>
+        <f t="shared" si="1"/>
+        <v>1225000</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2636,26 +2636,26 @@
         <v>22</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>621715.23750989977</v>
       </c>
       <c r="C23" s="2">
-        <f>B23*Rate</f>
+        <f t="shared" si="0"/>
         <v>43768.752720696946</v>
       </c>
       <c r="D23" s="2">
         <v>20500</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>685983.99023059674</v>
       </c>
       <c r="F23" s="2">
-        <v>49500</v>
+        <v>48500</v>
       </c>
       <c r="G23" s="3">
-        <f>F23*YearsOfSpending</f>
-        <v>1237500</v>
+        <f t="shared" si="1"/>
+        <v>1212500</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2663,26 +2663,26 @@
         <v>23</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>685983.99023059674</v>
       </c>
       <c r="C24" s="2">
-        <f>B24*Rate</f>
+        <f t="shared" si="0"/>
         <v>48293.272912234017</v>
       </c>
       <c r="D24" s="2">
         <v>21000</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>755277.26314283081</v>
       </c>
       <c r="F24" s="2">
-        <v>49000</v>
+        <v>48000</v>
       </c>
       <c r="G24" s="3">
-        <f>F24*YearsOfSpending</f>
-        <v>1225000</v>
+        <f t="shared" si="1"/>
+        <v>1200000</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2690,26 +2690,26 @@
         <v>24</v>
       </c>
       <c r="B25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>755277.26314283081</v>
       </c>
       <c r="C25" s="2">
-        <f>B25*Rate</f>
+        <f t="shared" si="0"/>
         <v>53171.519325255293</v>
       </c>
       <c r="D25" s="2">
         <v>21500</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>829948.78246808611</v>
       </c>
       <c r="F25" s="2">
-        <v>48500</v>
+        <v>47500</v>
       </c>
       <c r="G25" s="3">
-        <f>F25*YearsOfSpending</f>
-        <v>1212500</v>
+        <f t="shared" si="1"/>
+        <v>1187500</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2717,26 +2717,26 @@
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>829948.78246808611</v>
       </c>
       <c r="C26" s="2">
-        <f>B26*Rate</f>
+        <f t="shared" si="0"/>
         <v>58428.394285753267</v>
       </c>
       <c r="D26" s="2">
         <v>22000</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>910377.17675383936</v>
       </c>
       <c r="F26" s="2">
-        <v>48000</v>
+        <v>47000</v>
       </c>
       <c r="G26" s="3">
-        <f>F26*YearsOfSpending</f>
-        <v>1200000</v>
+        <f t="shared" si="1"/>
+        <v>1175000</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2744,26 +2744,26 @@
         <v>26</v>
       </c>
       <c r="B27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>910377.17675383936</v>
       </c>
       <c r="C27" s="2">
-        <f>B27*Rate</f>
+        <f t="shared" si="0"/>
         <v>64090.553243470298</v>
       </c>
       <c r="D27" s="2">
         <v>22500</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>996967.72999730962</v>
       </c>
       <c r="F27" s="2">
-        <v>47500</v>
+        <v>46500</v>
       </c>
       <c r="G27" s="3">
-        <f>F27*YearsOfSpending</f>
-        <v>1187500</v>
+        <f t="shared" si="1"/>
+        <v>1162500</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2771,26 +2771,26 @@
         <v>27</v>
       </c>
       <c r="B28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>996967.72999730962</v>
       </c>
       <c r="C28" s="2">
-        <f>B28*Rate</f>
+        <f t="shared" si="0"/>
         <v>70186.528191810605</v>
       </c>
       <c r="D28" s="2">
         <v>23000</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1090154.2581891203</v>
       </c>
       <c r="F28" s="2">
-        <v>47000</v>
+        <v>46000</v>
       </c>
       <c r="G28" s="3">
-        <f>F28*YearsOfSpending</f>
-        <v>1175000</v>
+        <f t="shared" si="1"/>
+        <v>1150000</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2798,26 +2798,26 @@
         <v>28</v>
       </c>
       <c r="B29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1090154.2581891203</v>
       </c>
       <c r="C29" s="2">
-        <f>B29*Rate</f>
+        <f t="shared" si="0"/>
         <v>76746.859776514073</v>
       </c>
       <c r="D29" s="2">
         <v>23500</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1190401.1179656344</v>
       </c>
       <c r="F29" s="2">
-        <v>46500</v>
+        <v>45500</v>
       </c>
       <c r="G29" s="3">
-        <f>F29*YearsOfSpending</f>
-        <v>1162500</v>
+        <f t="shared" si="1"/>
+        <v>1137500</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3020,7 +3020,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="8">
-        <f>LN(1+(Rate)*(YearsOfSpending*C2/A2))/LN(1+Rate)</f>
+        <f t="shared" ref="E2:E11" si="0">LN(1+(Rate)*(YearsOfSpending*C2/A2))/LN(1+Rate)</f>
         <v>46.640142106527392</v>
       </c>
     </row>
@@ -3039,7 +3039,7 @@
         <v>5.9999999999999991</v>
       </c>
       <c r="E3" s="8">
-        <f>LN(1+(Rate)*(YearsOfSpending*C3/A3))/LN(1+Rate)</f>
+        <f t="shared" si="0"/>
         <v>35.976247925771951</v>
       </c>
       <c r="G3" s="1"/>
@@ -3055,11 +3055,11 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="D4" s="6">
-        <f t="shared" ref="D4:D12" si="0">C4/A4</f>
+        <f t="shared" ref="D4:D11" si="1">C4/A4</f>
         <v>3.666666666666667</v>
       </c>
       <c r="E4" s="8">
-        <f>LN(1+(Rate)*(YearsOfSpending*C4/A4))/LN(1+Rate)</f>
+        <f t="shared" si="0"/>
         <v>29.525065304170056</v>
       </c>
     </row>
@@ -3074,11 +3074,11 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="E5" s="8">
-        <f>LN(1+(Rate)*(YearsOfSpending*C5/A5))/LN(1+Rate)</f>
+        <f t="shared" si="0"/>
         <v>24.788169989238295</v>
       </c>
     </row>
@@ -3093,11 +3093,11 @@
         <v>0.45</v>
       </c>
       <c r="D6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
       <c r="E6" s="8">
-        <f>LN(1+(Rate)*(YearsOfSpending*C6/A6))/LN(1+Rate)</f>
+        <f t="shared" si="0"/>
         <v>20.981709985429973</v>
       </c>
     </row>
@@ -3112,11 +3112,11 @@
         <v>0.4</v>
       </c>
       <c r="D7" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3333333333333335</v>
       </c>
       <c r="E7" s="8">
-        <f>LN(1+(Rate)*(YearsOfSpending*C7/A7))/LN(1+Rate)</f>
+        <f t="shared" si="0"/>
         <v>17.755725817126002</v>
       </c>
     </row>
@@ -3131,11 +3131,11 @@
         <v>0.35</v>
       </c>
       <c r="D8" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E8" s="8">
-        <f>LN(1+(Rate)*(YearsOfSpending*C8/A8))/LN(1+Rate)</f>
+        <f t="shared" si="0"/>
         <v>14.922750405019054</v>
       </c>
     </row>
@@ -3150,11 +3150,11 @@
         <v>0.3</v>
       </c>
       <c r="D9" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.74999999999999989</v>
       </c>
       <c r="E9" s="8">
-        <f>LN(1+(Rate)*(YearsOfSpending*C9/A9))/LN(1+Rate)</f>
+        <f t="shared" si="0"/>
         <v>12.370092149187174</v>
       </c>
     </row>
@@ -3169,11 +3169,11 @@
         <v>0.25</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.55555555555555558</v>
       </c>
       <c r="E10" s="8">
-        <f>LN(1+(Rate)*(YearsOfSpending*C10/A10))/LN(1+Rate)</f>
+        <f t="shared" si="0"/>
         <v>10.024249854356896</v>
       </c>
     </row>
@@ -3188,11 +3188,11 @@
         <v>0.2</v>
       </c>
       <c r="D11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="E11" s="8">
-        <f>LN(1+(Rate)*(YearsOfSpending*C11/A11))/LN(1+Rate)</f>
+        <f t="shared" si="0"/>
         <v>7.8341841092720275</v>
       </c>
     </row>

</xml_diff>